<commit_message>
table categories and stacked figures
</commit_message>
<xml_diff>
--- a/results/categorisation.xlsx
+++ b/results/categorisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kauane Bordin\Meu Drive (kauanembordin@gmail.com)\Capítulo Functional Traits\plant_functional_traits_chapter\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A172A17-EF04-4DA8-84FD-24D1CABE874F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD798C1-952D-4939-BD10-20F285805844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{31123227-CE7B-4451-B254-B9C15BAA26E2}"/>
   </bookViews>
@@ -41,12 +41,6 @@
     <t>Grassland</t>
   </si>
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Key-words included</t>
-  </si>
-  <si>
     <t>Forest</t>
   </si>
   <si>
@@ -138,6 +132,12 @@
   </si>
   <si>
     <t>"grassland", "grasslands", "steppe", "meadow-steppes"</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Words included</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,26 +507,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -534,111 +534,111 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated codes and results
</commit_message>
<xml_diff>
--- a/results/categorisation.xlsx
+++ b/results/categorisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kauane Bordin\Meu Drive (kauanembordin@gmail.com)\Capítulo Functional Traits\plant_functional_traits_chapter\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kauane\OneDrive\Área de Trabalho\plant_functional_traits_chapter\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2283A79-0A18-4AFF-AC5F-33575955770C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6F75F0-E67A-4051-A1B0-BFA04867ECE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{31123227-CE7B-4451-B254-B9C15BAA26E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31123227-CE7B-4451-B254-B9C15BAA26E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>Grassland</t>
-  </si>
-  <si>
-    <t>Forest</t>
-  </si>
-  <si>
-    <t>"forest", "forests","woodlands","shrublands"</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>LNC</t>
   </si>
@@ -53,9 +44,6 @@
     <t>"leaf N per area", "nitrogen fraction"</t>
   </si>
   <si>
-    <t>LC:LN</t>
-  </si>
-  <si>
     <t>"leaf C:N ratio", "leaf CN"</t>
   </si>
   <si>
@@ -77,15 +65,9 @@
     <t>"leaf seasonality", "deciduousness", "leaf longevity"</t>
   </si>
   <si>
-    <t>Growth</t>
-  </si>
-  <si>
     <t>"relative growth rate", "maximum growth rate"</t>
   </si>
   <si>
-    <t>Seeds</t>
-  </si>
-  <si>
     <t>Tree size</t>
   </si>
   <si>
@@ -98,52 +80,118 @@
     <t>Growth form</t>
   </si>
   <si>
-    <t>Tolerance</t>
-  </si>
-  <si>
     <t>"shade tolerance", "drought tolerance", "fire tolerance"</t>
   </si>
   <si>
+    <t>"pigment composition", "pigment concentration"</t>
+  </si>
+  <si>
+    <t>"leaf carbon per dry mass", "carbon fractions", "leaf carbon content"</t>
+  </si>
+  <si>
+    <t>"growth form", "growth habit"</t>
+  </si>
+  <si>
+    <t>"seed length", "seed mass"</t>
+  </si>
+  <si>
+    <t>"wood vessel length", "stem conduit density"</t>
+  </si>
+  <si>
+    <t>"root density", "root biomass", specific root length"</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>Traits used in this study</t>
+  </si>
+  <si>
+    <t>Traits obtained from the articles</t>
+  </si>
+  <si>
+    <t>LCC:LNC</t>
+  </si>
+  <si>
+    <t>Growth rate</t>
+  </si>
+  <si>
+    <t>Pigments</t>
+  </si>
+  <si>
+    <t>Seed size</t>
+  </si>
+  <si>
+    <t>"specific leaf area", "SLA", "LMA" (equals 1/SLA)</t>
+  </si>
+  <si>
+    <t>Root quantity</t>
+  </si>
+  <si>
+    <t>Stress tolerance</t>
+  </si>
+  <si>
+    <t>Vessel quantity</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>"leaf area"</t>
+  </si>
+  <si>
+    <t>LCC:LA</t>
+  </si>
+  <si>
+    <t>"leaf carbon content: leaf area ratio"</t>
+  </si>
+  <si>
+    <t>LDMC</t>
+  </si>
+  <si>
+    <t>LPC</t>
+  </si>
+  <si>
+    <t>"leaf phosphorus content"</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>"crown area", "crown cover"</t>
+  </si>
+  <si>
+    <t>"leaf dry-matter content", leaf mass"</t>
+  </si>
+  <si>
+    <t>LCaC</t>
+  </si>
+  <si>
+    <t>"leaf calcium content"</t>
+  </si>
+  <si>
+    <t>Trait class</t>
+  </si>
+  <si>
+    <t>"leaf thickness"</t>
+  </si>
+  <si>
+    <t>Crown size</t>
+  </si>
+  <si>
+    <t>Life history</t>
+  </si>
+  <si>
+    <t>Leaf</t>
+  </si>
+  <si>
+    <t>Stem</t>
+  </si>
+  <si>
     <t>Root</t>
   </si>
   <si>
-    <t>Vessel</t>
-  </si>
-  <si>
-    <t>Pigment</t>
-  </si>
-  <si>
-    <t>"pigment composition", "pigment concentration"</t>
-  </si>
-  <si>
-    <t>"leaf carbon per dry mass", "carbon fractions", "leaf carbon content"</t>
-  </si>
-  <si>
-    <t>"growth form", "growth habit"</t>
-  </si>
-  <si>
-    <t>"seed length", "seed mass"</t>
-  </si>
-  <si>
-    <t>"wood vessel length", "stem conduit density"</t>
-  </si>
-  <si>
-    <t>"root density", "root biomass", specific root length"</t>
-  </si>
-  <si>
-    <t>"grassland", "grasslands", "steppe", "meadow-steppes"</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Words included</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>"Specific leaf area"; "SLA", "LMA" (in the opposite effect)</t>
+    <t>Seed</t>
   </si>
 </sst>
 </file>
@@ -498,166 +546,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC405381-071A-4084-9E16-224C42CB87EE}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.7265625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
-    <sortCondition ref="A2:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+    <sortCondition ref="A2:A24"/>
+    <sortCondition ref="B2:B24"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>